<commit_message>
added eleemnts in the test_checklist
</commit_message>
<xml_diff>
--- a/test_checklist.xlsx
+++ b/test_checklist.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="71">
   <si>
     <t xml:space="preserve">Раздел</t>
   </si>
@@ -82,6 +82,9 @@
     <t xml:space="preserve">Навигация по главам свайпом и кнопками «вперёд/назад»</t>
   </si>
   <si>
+    <t xml:space="preserve">Ссылки работают</t>
+  </si>
+  <si>
     <t xml:space="preserve">Поиск внутри документа открывается и подсвечивает результаты</t>
   </si>
   <si>
@@ -91,12 +94,30 @@
     <t xml:space="preserve">Контекстное меню абзаца: Поделиться</t>
   </si>
   <si>
-    <t xml:space="preserve">Контекстное меню абзаца: Прослушать (TTS)</t>
+    <t xml:space="preserve">Контекстное меню абзаца: Прослушать (TTS) ОБА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Глава/Звук</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Настройки звука работают</t>
   </si>
   <si>
     <t xml:space="preserve">Контекстное меню абзаца: Заметка/выделение</t>
   </si>
   <si>
+    <t xml:space="preserve">Контекстное меню абзаца: Заметка очистка ошибка коректно работает</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Контекстное меню абзаца: Заметка добавление без выделения текста  ошибка коректно работает</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Контекстное меню абзаца: Заметка очистка работает</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Контекстное меню абзаца: Заметка добавление работает</t>
+  </si>
+  <si>
     <t xml:space="preserve">Проверить работу палитры цветов и сохранение выделений</t>
   </si>
   <si>
@@ -116,6 +137,9 @@
   </si>
   <si>
     <t xml:space="preserve">Удаление заметки требует подтверждения и отображает уведомление</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Экспорт в pdf работает</t>
   </si>
   <si>
     <t xml:space="preserve">Поиск</t>
@@ -250,7 +274,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -306,7 +329,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -317,6 +340,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -515,16 +542,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1048576"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="75.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="89.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.44"/>
   </cols>
   <sheetData>
@@ -703,10 +730,10 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C20" s="3"/>
     </row>
@@ -715,67 +742,67 @@
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="C26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>35</v>
@@ -784,7 +811,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>36</v>
@@ -793,34 +820,34 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="C30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>41</v>
@@ -829,7 +856,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>42</v>
@@ -838,7 +865,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>43</v>
@@ -847,7 +874,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>44</v>
@@ -901,25 +928,25 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="C42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>54</v>
@@ -928,7 +955,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>55</v>
@@ -937,7 +964,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>56</v>
@@ -946,46 +973,108 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="C47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>59</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="C49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="C50" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="3"/>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54" s="3"/>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>